<commit_message>
+ Add search by trade function
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -534,14 +534,14 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -552,13 +552,13 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -595,14 +595,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3">
+        <v>12345</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>12345</v>
       </c>
       <c r="D2" s="6">
         <v>12345</v>
@@ -639,14 +639,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="3">
+        <v>12345</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>12345</v>
       </c>
       <c r="D3" s="6">
         <v>12345</v>
@@ -684,14 +684,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="3">
+        <v>12346</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>12346</v>
       </c>
       <c r="D4" s="6">
         <v>12346</v>
@@ -728,14 +728,14 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="3">
+        <v>12346</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>12346</v>
       </c>
       <c r="D5" s="6">
         <v>12346</v>
@@ -773,14 +773,14 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="3">
+        <v>12347</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>12347</v>
       </c>
       <c r="D6" s="6">
         <v>12347</v>
@@ -817,14 +817,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="3">
+        <v>12347</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>3</v>
-      </c>
-      <c r="C7" s="3">
-        <v>12347</v>
       </c>
       <c r="D7" s="6">
         <v>12347</v>
@@ -862,14 +862,14 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="3">
+        <v>12348</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>4</v>
-      </c>
-      <c r="C8" s="3">
-        <v>12348</v>
       </c>
       <c r="D8" s="6">
         <v>12348</v>
@@ -906,14 +906,14 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="3">
+        <v>12348</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>4</v>
-      </c>
-      <c r="C9" s="3">
-        <v>12348</v>
       </c>
       <c r="D9" s="6">
         <v>12348</v>
@@ -951,14 +951,14 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="3">
+        <v>12349</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>12349</v>
       </c>
       <c r="D10" s="6">
         <v>12349</v>
@@ -995,14 +995,14 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="3">
+        <v>12349</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>5</v>
-      </c>
-      <c r="C11" s="3">
-        <v>12349</v>
       </c>
       <c r="D11" s="6">
         <v>12349</v>
@@ -1040,14 +1040,14 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="3">
+        <v>12350</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>6</v>
-      </c>
-      <c r="C12" s="3">
-        <v>12350</v>
       </c>
       <c r="D12" s="6">
         <v>12350</v>
@@ -1084,14 +1084,14 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="3">
+        <v>12350</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>6</v>
-      </c>
-      <c r="C13" s="3">
-        <v>12350</v>
       </c>
       <c r="D13" s="6">
         <v>12350</v>
@@ -1129,14 +1129,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="3">
+        <v>12351</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>12351</v>
       </c>
       <c r="D14" s="6">
         <v>12351</v>
@@ -1171,14 +1171,14 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="3">
+        <v>12351</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="3">
         <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>12351</v>
       </c>
       <c r="D15" s="6">
         <v>12351</v>
@@ -1214,14 +1214,14 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="3">
+        <v>12352</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3">
+      <c r="C16" s="3">
         <v>8</v>
-      </c>
-      <c r="C16" s="3">
-        <v>12352</v>
       </c>
       <c r="D16" s="6">
         <v>12352</v>
@@ -1256,14 +1256,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="3">
+        <v>12352</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3">
+      <c r="C17" s="3">
         <v>8</v>
-      </c>
-      <c r="C17" s="3">
-        <v>12352</v>
       </c>
       <c r="D17" s="6">
         <v>12352</v>
@@ -1299,14 +1299,14 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="3">
+        <v>12353</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
+      <c r="C18" s="3">
         <v>9</v>
-      </c>
-      <c r="C18" s="3">
-        <v>12353</v>
       </c>
       <c r="D18" s="6">
         <v>12353</v>
@@ -1341,14 +1341,14 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="3">
+        <v>12353</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="C19" s="3">
         <v>9</v>
-      </c>
-      <c r="C19" s="3">
-        <v>12353</v>
       </c>
       <c r="D19" s="6">
         <v>12353</v>
@@ -1384,14 +1384,14 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="3">
+        <v>12354</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="3">
+      <c r="C20" s="3">
         <v>10</v>
-      </c>
-      <c r="C20" s="3">
-        <v>12354</v>
       </c>
       <c r="D20" s="6">
         <v>12354</v>
@@ -1426,14 +1426,14 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="3">
+        <v>12354</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3">
+      <c r="C21" s="3">
         <v>10</v>
-      </c>
-      <c r="C21" s="3">
-        <v>12354</v>
       </c>
       <c r="D21" s="6">
         <v>12354</v>
@@ -1469,14 +1469,14 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="3">
+        <v>12355</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3">
+      <c r="C22" s="3">
         <v>11</v>
-      </c>
-      <c r="C22" s="3">
-        <v>12355</v>
       </c>
       <c r="D22" s="6">
         <v>12355</v>
@@ -1511,14 +1511,14 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="3">
+        <v>12355</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="3">
+      <c r="C23" s="3">
         <v>11</v>
-      </c>
-      <c r="C23" s="3">
-        <v>12355</v>
       </c>
       <c r="D23" s="6">
         <v>12355</v>
@@ -1554,14 +1554,14 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="3">
+        <v>12356</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="3">
+      <c r="C24" s="3">
         <v>12</v>
-      </c>
-      <c r="C24" s="3">
-        <v>12356</v>
       </c>
       <c r="D24" s="6">
         <v>12356</v>
@@ -1596,14 +1596,14 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="3">
+        <v>12356</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="3">
+      <c r="C25" s="3">
         <v>12</v>
-      </c>
-      <c r="C25" s="3">
-        <v>12356</v>
       </c>
       <c r="D25" s="6">
         <v>12356</v>
@@ -1639,14 +1639,14 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="3">
+        <v>12357</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="3">
+      <c r="C26" s="3">
         <v>13</v>
-      </c>
-      <c r="C26" s="3">
-        <v>12357</v>
       </c>
       <c r="D26" s="6">
         <v>12357</v>
@@ -1681,14 +1681,14 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="3">
+        <v>12357</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="3">
+      <c r="C27" s="3">
         <v>13</v>
-      </c>
-      <c r="C27" s="3">
-        <v>12357</v>
       </c>
       <c r="D27" s="6">
         <v>12357</v>
@@ -1724,14 +1724,14 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="3">
+        <v>12358</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="3">
+      <c r="C28" s="3">
         <v>14</v>
-      </c>
-      <c r="C28" s="3">
-        <v>12358</v>
       </c>
       <c r="D28" s="6">
         <v>12358</v>
@@ -1766,14 +1766,14 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="3">
+        <v>12358</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="3">
+      <c r="C29" s="3">
         <v>14</v>
-      </c>
-      <c r="C29" s="3">
-        <v>12358</v>
       </c>
       <c r="D29" s="6">
         <v>12358</v>
@@ -1809,14 +1809,14 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="3">
+        <v>12359</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="3">
+      <c r="C30" s="3">
         <v>15</v>
-      </c>
-      <c r="C30" s="3">
-        <v>12359</v>
       </c>
       <c r="D30" s="6">
         <v>12359</v>
@@ -1851,14 +1851,14 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="3">
+        <v>12359</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="3">
+      <c r="C31" s="3">
         <v>15</v>
-      </c>
-      <c r="C31" s="3">
-        <v>12359</v>
       </c>
       <c r="D31" s="6">
         <v>12359</v>
@@ -1894,14 +1894,14 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="3">
+        <v>12360</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="3">
+      <c r="C32" s="3">
         <v>16</v>
-      </c>
-      <c r="C32" s="3">
-        <v>12360</v>
       </c>
       <c r="D32" s="6">
         <v>12360</v>
@@ -1936,14 +1936,14 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="3">
+        <v>12360</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="3">
+      <c r="C33" s="3">
         <v>16</v>
-      </c>
-      <c r="C33" s="3">
-        <v>12360</v>
       </c>
       <c r="D33" s="6">
         <v>12360</v>
@@ -1979,14 +1979,14 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="3">
+        <v>12361</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="3">
+      <c r="C34" s="3">
         <v>17</v>
-      </c>
-      <c r="C34" s="3">
-        <v>12361</v>
       </c>
       <c r="D34" s="6">
         <v>12361</v>
@@ -2021,14 +2021,14 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="3">
+        <v>12361</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="3">
+      <c r="C35" s="3">
         <v>17</v>
-      </c>
-      <c r="C35" s="3">
-        <v>12361</v>
       </c>
       <c r="D35" s="6">
         <v>12361</v>
@@ -2064,14 +2064,14 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="3">
+        <v>12362</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="3">
-        <v>18</v>
-      </c>
       <c r="C36" s="3">
-        <v>12362</v>
+        <v>18</v>
       </c>
       <c r="D36" s="6">
         <v>12362</v>
@@ -2106,14 +2106,14 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="3">
+        <v>12362</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="3">
-        <v>18</v>
-      </c>
       <c r="C37" s="3">
-        <v>12362</v>
+        <v>18</v>
       </c>
       <c r="D37" s="6">
         <v>12362</v>
@@ -2149,14 +2149,14 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="3">
+        <v>12363</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="3">
+      <c r="C38" s="3">
         <v>19</v>
-      </c>
-      <c r="C38" s="3">
-        <v>12363</v>
       </c>
       <c r="D38" s="6">
         <v>12363</v>
@@ -2191,14 +2191,14 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="3">
+        <v>12363</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="3">
+      <c r="C39" s="3">
         <v>19</v>
-      </c>
-      <c r="C39" s="3">
-        <v>12363</v>
       </c>
       <c r="D39" s="6">
         <v>12363</v>

</xml_diff>

<commit_message>
* Update fix error
* Change return string of issue in ConvOjb
* Change search method
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\workspace2\AutoTagging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11122_000\workspace\Autotag\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -112,8 +112,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +125,18 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -171,20 +183,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{9D8874FA-42AA-4A5F-B1B5-99100653D31C}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -534,20 +575,21 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -604,37 +646,37 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>12345</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="6">
         <v>208.92707407879897</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="6">
         <v>35.605843256192806</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>95.103371849872815</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>78.217858972733339</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>69.857324382051161</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>44.092825461891941</v>
       </c>
     </row>
@@ -648,38 +690,37 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>12345</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="4">
-        <f>J3+K3+L3</f>
+      <c r="I3" s="6">
         <v>213.32123082260614</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="6">
         <v>40</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>95.103371849872815</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>78.217858972733339</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>69.857324382051161</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>44.092825461891941</v>
       </c>
     </row>
@@ -693,37 +734,37 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>12346</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>92.578968827717375</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>58.064374913844453</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>3.704547002928138</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>30.810046910944777</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>6.7987797240415482</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>77.618307021074813</v>
       </c>
     </row>
@@ -737,38 +778,37 @@
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>12346</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="6">
-        <f t="shared" ref="I5" si="0">J5+K5+L5</f>
+      <c r="I5" s="5">
         <v>92.578968827717375</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>58.064374913844453</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>3.704547002928138</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>30.810046910944777</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>6.7987797240415482</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>77.618307021074813</v>
       </c>
     </row>
@@ -782,37 +822,37 @@
       <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>12347</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="6">
         <v>139.18826406302765</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="6">
         <v>23.579468103127653</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>34.029123988591792</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>81.579671971308215</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>50.168934202593519</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>9.4519493035683517</v>
       </c>
     </row>
@@ -826,38 +866,37 @@
       <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>12347</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="4">
-        <f t="shared" ref="I7" si="1">J7+K7+L7</f>
+      <c r="I7" s="6">
         <v>140.60879595990002</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="6">
         <v>25</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>34.029123988591792</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>81.579671971308215</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>50.168934202593519</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <v>9.4519493035683517</v>
       </c>
     </row>
@@ -871,37 +910,37 @@
       <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>12348</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="7">
         <v>178.11407542762998</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="7">
         <v>70.119186047086231</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>14.75493269134347</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>93.23995668920027</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <v>44.62136265992811</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>27.503236632674486</v>
       </c>
     </row>
@@ -915,38 +954,37 @@
       <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>12348</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="5">
-        <f t="shared" ref="I9" si="2">J9+K9+L9</f>
+      <c r="I9" s="7">
         <v>182.99488938054373</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="7">
         <v>75</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>14.75493269134347</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>93.23995668920027</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>44.62136265992811</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>27.503236632674486</v>
       </c>
     </row>
@@ -960,37 +998,37 @@
       <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>12349</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>218.46694735523926</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>91.916404285568206</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>84.127452881745796</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>42.423090187925268</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="5">
         <v>38.073806962893528</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <v>36.695113451472714</v>
       </c>
     </row>
@@ -1004,38 +1042,37 @@
       <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>12349</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="6">
-        <f t="shared" ref="I11" si="3">J11+K11+L11</f>
+      <c r="I11" s="5">
         <v>218.46694735523926</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>91.916404285568206</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>84.127452881745796</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>42.423090187925268</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>38.073806962893528</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <v>36.695113451472714</v>
       </c>
     </row>
@@ -1049,37 +1086,37 @@
       <c r="C12" s="3">
         <v>6</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>12350</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="7">
         <v>235.57968677886589</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="7">
         <v>90.890533527990897</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>61.320268642398304</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <v>83.368884608476677</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <v>62.06717311761755</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <v>71.265346617354027</v>
       </c>
     </row>
@@ -1093,38 +1130,37 @@
       <c r="C13" s="3">
         <v>6</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>12350</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="5">
-        <f t="shared" ref="I13" si="4">J13+K13+L13</f>
+      <c r="I13" s="7">
         <v>239.68915325087499</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="7">
         <v>95</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>61.320268642398304</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>83.368884608476677</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <v>62.06717311761755</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>71.265346617354027</v>
       </c>
     </row>
@@ -1138,35 +1174,35 @@
       <c r="C14" s="3">
         <v>7</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>12351</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="6">
         <v>120.09273916096612</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="6">
         <v>80.435461860448001</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>28.191257892194798</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="6">
         <v>11.466019408323325</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="6">
         <v>53.810181727259291</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="6">
         <v>6.4586922852102209</v>
       </c>
     </row>
@@ -1180,36 +1216,35 @@
       <c r="C15" s="3">
         <v>7</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>12351</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="4">
-        <f t="shared" ref="I15" si="5">J15+K15+L15</f>
+      <c r="I15" s="6">
         <v>123.1912578921948</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="6">
         <v>80</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>28.191257892194798</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="6">
         <v>15</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="6">
         <v>55</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="6">
         <v>7</v>
       </c>
     </row>
@@ -1223,35 +1258,35 @@
       <c r="C16" s="3">
         <v>8</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>12352</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="7">
         <v>124.49781857558426</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>18.22506903815999</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>83.025626021112004</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="7">
         <v>23.247123516312275</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="7">
         <v>10.713386681647474</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="7">
         <v>50.717570436078852</v>
       </c>
     </row>
@@ -1265,36 +1300,35 @@
       <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>12352</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="5">
-        <f t="shared" ref="I17" si="6">J17+K17+L17</f>
+      <c r="I17" s="7">
         <v>126.25069505927199</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>18.22506903815999</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>83.025626021112004</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="7">
         <v>25</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="7">
         <v>11</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="7">
         <v>52</v>
       </c>
     </row>
@@ -1308,35 +1342,35 @@
       <c r="C18" s="3">
         <v>9</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>12353</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="6">
         <v>139.33897382053257</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="6">
         <v>52.628097250439644</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>22.793023330880235</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="6">
         <v>63.917853239212683</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="6">
         <v>33.764455498926971</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="6">
         <v>66.442605186829169</v>
       </c>
     </row>
@@ -1350,36 +1384,35 @@
       <c r="C19" s="3">
         <v>9</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>12353</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="5"/>
+      <c r="H19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="4">
-        <f t="shared" ref="I19" si="7">J19+K19+L19</f>
+      <c r="I19" s="6">
         <v>139.79302333088023</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="6">
         <v>52</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>22.793023330880235</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="6">
         <v>65</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="6">
         <v>34</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19" s="6">
         <v>67</v>
       </c>
     </row>
@@ -1393,35 +1426,35 @@
       <c r="C20" s="3">
         <v>10</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>12354</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="7">
         <v>264.71247656308799</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>96.846582836184936</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>73.446307218460134</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="7">
         <v>94.419586508442919</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="7">
         <v>79.443051948320075</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="7">
         <v>41.715948669600941</v>
       </c>
     </row>
@@ -1435,36 +1468,35 @@
       <c r="C21" s="3">
         <v>10</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>12354</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="5">
-        <f t="shared" ref="I21" si="8">J21+K21+L21</f>
+      <c r="I21" s="7">
         <v>266.29289005464506</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>96.846582836184936</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>73.446307218460134</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="7">
         <v>96</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="7">
         <v>98</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="7">
         <v>43</v>
       </c>
     </row>
@@ -1478,35 +1510,35 @@
       <c r="C22" s="3">
         <v>11</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>12355</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>50.674686728653015</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>10.534133927078205</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>34.975462551551331</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="5">
         <v>5.1650902500234857</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="5">
         <v>1.7302466281576723</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="5">
         <v>76.816661368132088</v>
       </c>
     </row>
@@ -1520,36 +1552,35 @@
       <c r="C23" s="3">
         <v>11</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>12355</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="6">
-        <f t="shared" ref="I23" si="9">J23+K23+L23</f>
+      <c r="I23" s="5">
         <v>50.674686728653015</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <v>10.534133927078205</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>34.975462551551331</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="5">
         <v>5.1650902500234857</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="5">
         <v>1.7302466281576723</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="5">
         <v>76.816661368132088</v>
       </c>
     </row>
@@ -1563,35 +1594,35 @@
       <c r="C24" s="3">
         <v>12</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>12356</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="7">
         <v>157.22639983855399</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="5">
         <v>11.411121767886367</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="5">
         <v>89.373248793898171</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="7">
         <v>56.442029276769453</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="7">
         <v>42.252865028965495</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="7">
         <v>72.894493040276174</v>
       </c>
     </row>
@@ -1605,36 +1636,35 @@
       <c r="C25" s="3">
         <v>12</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>12356</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="E25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="5">
-        <f t="shared" ref="I25" si="10">J25+K25+L25</f>
+      <c r="I25" s="7">
         <v>156.78437056178456</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="5">
         <v>11.411121767886367</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="5">
         <v>89.373248793898171</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="7">
         <v>56</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="7">
         <v>44</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="7">
         <v>75</v>
       </c>
     </row>
@@ -1648,35 +1678,35 @@
       <c r="C26" s="3">
         <v>13</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>12357</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="6">
         <v>114.98296045734511</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="5">
         <v>33.061583954292281</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="5">
         <v>49.124320547387015</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="6">
         <v>32.797055955665833</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="6">
         <v>28.429042401895277</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N26" s="6">
         <v>20.237229940974309</v>
       </c>
     </row>
@@ -1690,36 +1720,35 @@
       <c r="C27" s="3">
         <v>13</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>12357</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="4">
-        <f t="shared" ref="I27" si="11">J27+K27+L27</f>
+      <c r="I27" s="6">
         <v>115.18590450167929</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="5">
         <v>33.061583954292281</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="5">
         <v>49.124320547387015</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="6">
         <v>33</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27" s="6">
         <v>30</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27" s="6">
         <v>23</v>
       </c>
     </row>
@@ -1733,35 +1762,35 @@
       <c r="C28" s="3">
         <v>14</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>12358</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="5">
         <v>200.89090114992351</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="5">
         <v>72.015411896894292</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="5">
         <v>41.887839110038904</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L28" s="5">
         <v>86.987650142990304</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="5">
         <v>58.722014816697254</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="5">
         <v>78.996379370783941</v>
       </c>
     </row>
@@ -1775,36 +1804,35 @@
       <c r="C29" s="3">
         <v>14</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>12358</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="6">
-        <f t="shared" ref="I29" si="12">J29+K29+L29</f>
+      <c r="I29" s="5">
         <v>200.89090114992351</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="5">
         <v>72.015411896894292</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="5">
         <v>41.887839110038904</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L29" s="5">
         <v>86.987650142990304</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M29" s="5">
         <v>58.722014816697254</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="5">
         <v>78.996379370783941</v>
       </c>
     </row>
@@ -1818,35 +1846,35 @@
       <c r="C30" s="3">
         <v>15</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>12359</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6" t="s">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>141.25200003109654</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="5">
         <v>38.584605923877604</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="5">
         <v>8.9002966731389961</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L30" s="5">
         <v>93.767097434079943</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M30" s="5">
         <v>7.8920670111144675</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="5">
         <v>67.214034479482251</v>
       </c>
     </row>
@@ -1860,36 +1888,35 @@
       <c r="C31" s="3">
         <v>15</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>12359</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="6">
-        <f t="shared" ref="I31" si="13">J31+K31+L31</f>
+      <c r="I31" s="5">
         <v>141.25200003109654</v>
       </c>
-      <c r="J31" s="6">
+      <c r="J31" s="5">
         <v>38.584605923877604</v>
       </c>
-      <c r="K31" s="6">
+      <c r="K31" s="5">
         <v>8.9002966731389961</v>
       </c>
-      <c r="L31" s="6">
+      <c r="L31" s="5">
         <v>93.767097434079943</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="5">
         <v>7.8920670111144675</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="5">
         <v>67.214034479482251</v>
       </c>
     </row>
@@ -1903,35 +1930,35 @@
       <c r="C32" s="3">
         <v>16</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>12360</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6" t="s">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="5">
         <v>188.3666103030879</v>
       </c>
-      <c r="J32" s="6">
+      <c r="J32" s="5">
         <v>96.275832974123361</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="5">
         <v>71.855371931744628</v>
       </c>
-      <c r="L32" s="6">
+      <c r="L32" s="5">
         <v>20.235405397219907</v>
       </c>
-      <c r="M32" s="6">
+      <c r="M32" s="5">
         <v>7.3575033337787694</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32" s="5">
         <v>53.316255126737801</v>
       </c>
     </row>
@@ -1945,36 +1972,35 @@
       <c r="C33" s="3">
         <v>16</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>12360</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="6">
-        <f t="shared" ref="I33" si="14">J33+K33+L33</f>
+      <c r="I33" s="5">
         <v>188.3666103030879</v>
       </c>
-      <c r="J33" s="6">
+      <c r="J33" s="5">
         <v>96.275832974123361</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K33" s="5">
         <v>71.855371931744628</v>
       </c>
-      <c r="L33" s="6">
+      <c r="L33" s="5">
         <v>20.235405397219907</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="5">
         <v>7.3575033337787694</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="5">
         <v>53.316255126737801</v>
       </c>
     </row>
@@ -1988,35 +2014,35 @@
       <c r="C34" s="3">
         <v>17</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>12361</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6" t="s">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="5">
         <v>100.54279648387319</v>
       </c>
-      <c r="J34" s="6">
+      <c r="J34" s="5">
         <v>3.9681914194773404</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K34" s="5">
         <v>37.940421132831517</v>
       </c>
-      <c r="L34" s="6">
+      <c r="L34" s="5">
         <v>58.63418393156433</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34" s="5">
         <v>69.292528396007867</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="5">
         <v>21.724663135751921</v>
       </c>
     </row>
@@ -2030,36 +2056,35 @@
       <c r="C35" s="3">
         <v>17</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>12361</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6" t="s">
+      <c r="G35" s="5"/>
+      <c r="H35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="6">
-        <f t="shared" ref="I35" si="15">J35+K35+L35</f>
+      <c r="I35" s="5">
         <v>100.54279648387319</v>
       </c>
-      <c r="J35" s="6">
+      <c r="J35" s="5">
         <v>3.9681914194773404</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K35" s="5">
         <v>37.940421132831517</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L35" s="5">
         <v>58.63418393156433</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="5">
         <v>69.292528396007867</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="5">
         <v>21.724663135751921</v>
       </c>
     </row>
@@ -2073,35 +2098,35 @@
       <c r="C36" s="3">
         <v>18</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>12362</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6" t="s">
+      <c r="G36" s="5"/>
+      <c r="H36" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="5">
         <v>118.05007256379093</v>
       </c>
-      <c r="J36" s="6">
+      <c r="J36" s="5">
         <v>11.618527006790657</v>
       </c>
-      <c r="K36" s="6">
+      <c r="K36" s="5">
         <v>77.533241552769667</v>
       </c>
-      <c r="L36" s="6">
+      <c r="L36" s="5">
         <v>28.898304004230603</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="5">
         <v>12.960015791662261</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="5">
         <v>54.484842238223074</v>
       </c>
     </row>
@@ -2115,36 +2140,35 @@
       <c r="C37" s="3">
         <v>18</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>12362</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6" t="s">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="6">
-        <f t="shared" ref="I37" si="16">J37+K37+L37</f>
+      <c r="I37" s="5">
         <v>118.05007256379093</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37" s="5">
         <v>11.618527006790657</v>
       </c>
-      <c r="K37" s="6">
+      <c r="K37" s="5">
         <v>77.533241552769667</v>
       </c>
-      <c r="L37" s="6">
+      <c r="L37" s="5">
         <v>28.898304004230603</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="5">
         <v>12.960015791662261</v>
       </c>
-      <c r="N37" s="6">
+      <c r="N37" s="5">
         <v>54.484842238223074</v>
       </c>
     </row>
@@ -2158,35 +2182,35 @@
       <c r="C38" s="3">
         <v>19</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>12363</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6" t="s">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="5">
         <v>155.09630929862217</v>
       </c>
-      <c r="J38" s="6">
+      <c r="J38" s="5">
         <v>84.931795684514057</v>
       </c>
-      <c r="K38" s="6">
+      <c r="K38" s="5">
         <v>44.046715963956018</v>
       </c>
-      <c r="L38" s="6">
+      <c r="L38" s="5">
         <v>26.117797650152074</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="5">
         <v>68.855485594706408</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="5">
         <v>87.94490937202049</v>
       </c>
     </row>
@@ -2200,36 +2224,35 @@
       <c r="C39" s="3">
         <v>19</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>12363</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6" t="s">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="6">
-        <f t="shared" ref="I39" si="17">J39+K39+L39</f>
+      <c r="I39" s="5">
         <v>155.09630929862217</v>
       </c>
-      <c r="J39" s="6">
+      <c r="J39" s="5">
         <v>84.931795684514057</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K39" s="5">
         <v>44.046715963956018</v>
       </c>
-      <c r="L39" s="6">
+      <c r="L39" s="5">
         <v>26.117797650152074</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39" s="5">
         <v>68.855485594706408</v>
       </c>
-      <c r="N39" s="6">
+      <c r="N39" s="5">
         <v>87.94490937202049</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create process to import trade/issue from User file
+ Add class ImportTagProcess
* Update to fix bug of method getIssuebyID
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,21 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="28">
   <si>
-    <t>TRN_NB</t>
-  </si>
-  <si>
-    <t>FAM</t>
-  </si>
-  <si>
-    <t>GROUP</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
     <t>PL</t>
   </si>
   <si>
@@ -110,6 +95,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>M_NB</t>
+  </si>
+  <si>
+    <t>M_TRN_FMLY</t>
+  </si>
+  <si>
+    <t>M_TRN_GRP</t>
+  </si>
+  <si>
+    <t>M_TRN_TYPE</t>
+  </si>
+  <si>
+    <t>M_TP_FXBASE</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -195,6 +195,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +562,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +579,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +588,7 @@
     <col min="2" max="2" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -597,46 +598,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -644,7 +645,7 @@
         <v>12345</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -653,16 +654,16 @@
         <v>12345</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I2" s="6">
         <v>208.92707407879897</v>
@@ -688,7 +689,7 @@
         <v>12345</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -697,16 +698,16 @@
         <v>12345</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I3" s="6">
         <v>213.32123082260614</v>
@@ -732,7 +733,7 @@
         <v>12346</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -741,16 +742,16 @@
         <v>12346</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I4" s="5">
         <v>92.578968827717375</v>
@@ -776,7 +777,7 @@
         <v>12346</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -785,16 +786,16 @@
         <v>12346</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5">
         <v>92.578968827717375</v>
@@ -820,7 +821,7 @@
         <v>12347</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>3</v>
@@ -829,16 +830,16 @@
         <v>12347</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I6" s="6">
         <v>139.18826406302765</v>
@@ -864,7 +865,7 @@
         <v>12347</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
@@ -873,16 +874,16 @@
         <v>12347</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I7" s="6">
         <v>140.60879595990002</v>
@@ -908,7 +909,7 @@
         <v>12348</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
@@ -917,16 +918,16 @@
         <v>12348</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I8" s="7">
         <v>178.11407542762998</v>
@@ -952,7 +953,7 @@
         <v>12348</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>4</v>
@@ -961,16 +962,16 @@
         <v>12348</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I9" s="7">
         <v>182.99488938054373</v>
@@ -996,7 +997,7 @@
         <v>12349</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
@@ -1005,16 +1006,16 @@
         <v>12349</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5">
         <v>218.46694735523926</v>
@@ -1040,7 +1041,7 @@
         <v>12349</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
@@ -1049,16 +1050,16 @@
         <v>12349</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I11" s="5">
         <v>218.46694735523926</v>
@@ -1084,7 +1085,7 @@
         <v>12350</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <v>6</v>
@@ -1093,16 +1094,16 @@
         <v>12350</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I12" s="7">
         <v>235.57968677886589</v>
@@ -1128,7 +1129,7 @@
         <v>12350</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3">
         <v>6</v>
@@ -1137,16 +1138,16 @@
         <v>12350</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I13" s="7">
         <v>239.68915325087499</v>
@@ -1172,7 +1173,7 @@
         <v>12351</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3">
         <v>7</v>
@@ -1181,16 +1182,16 @@
         <v>12351</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I14" s="6">
         <v>120.09273916096612</v>
@@ -1216,7 +1217,7 @@
         <v>12351</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3">
         <v>7</v>
@@ -1225,16 +1226,16 @@
         <v>12351</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I15" s="6">
         <v>123.1912578921948</v>
@@ -1260,7 +1261,7 @@
         <v>12352</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3">
         <v>8</v>
@@ -1269,16 +1270,16 @@
         <v>12352</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G16" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I16" s="7">
         <v>124.49781857558426</v>
@@ -1304,7 +1305,7 @@
         <v>12352</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3">
         <v>8</v>
@@ -1313,16 +1314,16 @@
         <v>12352</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I17" s="7">
         <v>126.25069505927199</v>
@@ -1348,7 +1349,7 @@
         <v>12353</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3">
         <v>9</v>
@@ -1357,16 +1358,16 @@
         <v>12353</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G18" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I18" s="6">
         <v>139.33897382053257</v>
@@ -1392,7 +1393,7 @@
         <v>12353</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3">
         <v>9</v>
@@ -1401,16 +1402,16 @@
         <v>12353</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I19" s="6">
         <v>139.79302333088023</v>
@@ -1436,7 +1437,7 @@
         <v>12354</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C20" s="3">
         <v>10</v>
@@ -1445,16 +1446,16 @@
         <v>12354</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G20" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I20" s="7">
         <v>264.71247656308799</v>
@@ -1480,7 +1481,7 @@
         <v>12354</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C21" s="3">
         <v>10</v>
@@ -1489,16 +1490,16 @@
         <v>12354</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I21" s="7">
         <v>266.29289005464506</v>
@@ -1524,7 +1525,7 @@
         <v>12355</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3">
         <v>11</v>
@@ -1533,16 +1534,16 @@
         <v>12355</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G22" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I22" s="5">
         <v>50.674686728653015</v>
@@ -1568,7 +1569,7 @@
         <v>12355</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3">
         <v>11</v>
@@ -1577,16 +1578,16 @@
         <v>12355</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I23" s="5">
         <v>50.674686728653015</v>
@@ -1612,7 +1613,7 @@
         <v>12356</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3">
         <v>12</v>
@@ -1621,16 +1622,16 @@
         <v>12356</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G24" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I24" s="7">
         <v>157.22639983855399</v>
@@ -1656,7 +1657,7 @@
         <v>12356</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3">
         <v>12</v>
@@ -1665,16 +1666,16 @@
         <v>12356</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G25" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I25" s="7">
         <v>156.78437056178456</v>
@@ -1700,7 +1701,7 @@
         <v>12357</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3">
         <v>13</v>
@@ -1709,16 +1710,16 @@
         <v>12357</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I26" s="6">
         <v>114.98296045734511</v>
@@ -1744,7 +1745,7 @@
         <v>12357</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C27" s="3">
         <v>13</v>
@@ -1753,16 +1754,16 @@
         <v>12357</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I27" s="6">
         <v>115.18590450167929</v>
@@ -1788,7 +1789,7 @@
         <v>12358</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3">
         <v>14</v>
@@ -1797,16 +1798,16 @@
         <v>12358</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I28" s="5">
         <v>200.89090114992351</v>
@@ -1832,7 +1833,7 @@
         <v>12358</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C29" s="3">
         <v>14</v>
@@ -1841,16 +1842,16 @@
         <v>12358</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I29" s="5">
         <v>200.89090114992351</v>
@@ -1876,7 +1877,7 @@
         <v>12359</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3">
         <v>15</v>
@@ -1885,16 +1886,16 @@
         <v>12359</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I30" s="5">
         <v>141.25200003109654</v>
@@ -1920,7 +1921,7 @@
         <v>12359</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C31" s="3">
         <v>15</v>
@@ -1929,16 +1930,16 @@
         <v>12359</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I31" s="5">
         <v>141.25200003109654</v>
@@ -1964,7 +1965,7 @@
         <v>12360</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3">
         <v>16</v>
@@ -1973,16 +1974,16 @@
         <v>12360</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I32" s="5">
         <v>188.3666103030879</v>
@@ -2008,7 +2009,7 @@
         <v>12360</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C33" s="3">
         <v>16</v>
@@ -2017,16 +2018,16 @@
         <v>12360</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I33" s="5">
         <v>188.3666103030879</v>
@@ -2052,7 +2053,7 @@
         <v>12361</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3">
         <v>17</v>
@@ -2061,16 +2062,16 @@
         <v>12361</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I34" s="5">
         <v>100.54279648387319</v>
@@ -2096,7 +2097,7 @@
         <v>12361</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3">
         <v>17</v>
@@ -2105,16 +2106,16 @@
         <v>12361</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I35" s="5">
         <v>100.54279648387319</v>
@@ -2140,7 +2141,7 @@
         <v>12362</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C36" s="3">
         <v>18</v>
@@ -2149,16 +2150,16 @@
         <v>12362</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I36" s="5">
         <v>118.05007256379093</v>
@@ -2184,7 +2185,7 @@
         <v>12362</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C37" s="3">
         <v>18</v>
@@ -2193,16 +2194,16 @@
         <v>12362</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I37" s="5">
         <v>118.05007256379093</v>
@@ -2228,7 +2229,7 @@
         <v>12363</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C38" s="3">
         <v>19</v>
@@ -2237,16 +2238,16 @@
         <v>12363</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I38" s="5">
         <v>155.09630929862217</v>
@@ -2272,7 +2273,7 @@
         <v>12363</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C39" s="3">
         <v>19</v>
@@ -2281,16 +2282,16 @@
         <v>12363</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I39" s="5">
         <v>155.09630929862217</v>

</xml_diff>

<commit_message>
Update function for Scene 2
+ Add function to process non-trade key value .
* Change MajorProc to GetTagByTrade
* Modify MajorProc to process corresponding key value.
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -97,19 +97,19 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>M_NB</t>
-  </si>
-  <si>
-    <t>M_TRN_FMLY</t>
-  </si>
-  <si>
-    <t>M_TRN_GRP</t>
-  </si>
-  <si>
-    <t>M_TRN_TYPE</t>
-  </si>
-  <si>
-    <t>M_TP_FXBASE</t>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>TRN_FMLY</t>
+  </si>
+  <si>
+    <t>TRN_GRP</t>
+  </si>
+  <si>
+    <t>TRN_TYPE</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>